<commit_message>
Update analyses and scripts
</commit_message>
<xml_diff>
--- a/data/Adverse-events-dose-v5.xlsx
+++ b/data/Adverse-events-dose-v5.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mickaeleskinazi/Documents/GitHub/metaanalysis-psychedelics/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02799259-B5A0-B546-ADF0-64F99A5C2773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA8C5C83-CEE7-3948-87C8-FBF08FE60706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18400" yWindow="1920" windowWidth="27640" windowHeight="16940" xr2:uid="{C942188B-0665-D64B-B3EA-6E2D21234088}"/>
+    <workbookView xWindow="1760" yWindow="1440" windowWidth="32440" windowHeight="16940" xr2:uid="{C942188B-0665-D64B-B3EA-6E2D21234088}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7491" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7959" uniqueCount="281">
   <si>
     <t>study_id</t>
   </si>
@@ -869,12 +869,24 @@
   <si>
     <t>hypoglycemia</t>
   </si>
+  <si>
+    <t>followup</t>
+  </si>
+  <si>
+    <t>impaired gait/balance</t>
+  </si>
+  <si>
+    <t>Danforth2018</t>
+  </si>
+  <si>
+    <t>ISRS</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -914,6 +926,12 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1311,10 +1329,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A33BC1D5-BEC9-9348-8EA2-A2DED104290C}">
-  <dimension ref="A1:J1141"/>
+  <dimension ref="A1:J1213"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1142" sqref="J1142"/>
+    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
+      <selection activeCell="J996" sqref="J996"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -30568,7 +30586,7 @@
         <v>0</v>
       </c>
       <c r="J971" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
     </row>
     <row r="972" spans="1:10" x14ac:dyDescent="0.2">
@@ -30629,7 +30647,7 @@
         <v>0</v>
       </c>
       <c r="J973" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
     </row>
     <row r="974" spans="1:10" x14ac:dyDescent="0.2">
@@ -30690,7 +30708,7 @@
         <v>0</v>
       </c>
       <c r="J975" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
     </row>
     <row r="976" spans="1:10" x14ac:dyDescent="0.2">
@@ -30751,7 +30769,7 @@
         <v>0</v>
       </c>
       <c r="J977" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
     </row>
     <row r="978" spans="1:10" x14ac:dyDescent="0.2">
@@ -30812,7 +30830,7 @@
         <v>0</v>
       </c>
       <c r="J979" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
     </row>
     <row r="980" spans="1:10" x14ac:dyDescent="0.2">
@@ -30873,7 +30891,7 @@
         <v>0</v>
       </c>
       <c r="J981" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
     </row>
     <row r="982" spans="1:10" x14ac:dyDescent="0.2">
@@ -30934,7 +30952,7 @@
         <v>0</v>
       </c>
       <c r="J983" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
     </row>
     <row r="984" spans="1:10" x14ac:dyDescent="0.2">
@@ -30995,7 +31013,7 @@
         <v>0</v>
       </c>
       <c r="J985" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
     </row>
     <row r="986" spans="1:10" x14ac:dyDescent="0.2">
@@ -31056,7 +31074,7 @@
         <v>0</v>
       </c>
       <c r="J987" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
     </row>
     <row r="988" spans="1:10" x14ac:dyDescent="0.2">
@@ -31117,7 +31135,7 @@
         <v>0</v>
       </c>
       <c r="J989" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
     </row>
     <row r="990" spans="1:10" x14ac:dyDescent="0.2">
@@ -31178,7 +31196,7 @@
         <v>0</v>
       </c>
       <c r="J991" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
     </row>
     <row r="992" spans="1:10" x14ac:dyDescent="0.2">
@@ -31239,7 +31257,7 @@
         <v>0</v>
       </c>
       <c r="J993" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
     </row>
     <row r="994" spans="1:10" x14ac:dyDescent="0.2">
@@ -31300,7 +31318,7 @@
         <v>0</v>
       </c>
       <c r="J995" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
     </row>
     <row r="996" spans="1:10" x14ac:dyDescent="0.2">
@@ -35720,7 +35738,2204 @@
         <v>273</v>
       </c>
     </row>
+    <row r="1142" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1142" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1142" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1142" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1142" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1142">
+        <v>4</v>
+      </c>
+      <c r="F1142" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1142" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1142">
+        <v>0.25</v>
+      </c>
+      <c r="I1142">
+        <v>0</v>
+      </c>
+      <c r="J1142" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="1143" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1143" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1143" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1143" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1143" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1143">
+        <v>8</v>
+      </c>
+      <c r="F1143" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1143" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1143">
+        <v>0.75</v>
+      </c>
+      <c r="I1143">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="1144" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1144" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1144" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1144" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1144" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1144">
+        <v>4</v>
+      </c>
+      <c r="F1144" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1144" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1144">
+        <v>0.25</v>
+      </c>
+      <c r="I1144">
+        <v>0</v>
+      </c>
+      <c r="J1144" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="1145" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1145" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1145" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1145" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1145" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1145">
+        <v>8</v>
+      </c>
+      <c r="F1145" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1145" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1145">
+        <v>0.625</v>
+      </c>
+      <c r="I1145">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="1146" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1146" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1146" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1146" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1146" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1146">
+        <v>4</v>
+      </c>
+      <c r="F1146" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1146" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1146">
+        <v>0.25</v>
+      </c>
+      <c r="I1146">
+        <v>0</v>
+      </c>
+      <c r="J1146" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="1147" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1147" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1147" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1147" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1147" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1147">
+        <v>8</v>
+      </c>
+      <c r="F1147" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1147" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1147">
+        <v>0.5</v>
+      </c>
+      <c r="I1147">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="1148" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1148" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1148" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1148" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1148" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1148">
+        <v>4</v>
+      </c>
+      <c r="F1148" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1148" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1148">
+        <v>0.25</v>
+      </c>
+      <c r="I1148">
+        <v>0</v>
+      </c>
+      <c r="J1148" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="1149" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1149" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1149" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1149" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1149" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1149">
+        <v>8</v>
+      </c>
+      <c r="F1149" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1149" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1149">
+        <v>0.5</v>
+      </c>
+      <c r="I1149">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="1150" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1150" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1150" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1150" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1150" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1150">
+        <v>4</v>
+      </c>
+      <c r="F1150" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1150" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1150">
+        <v>0.25</v>
+      </c>
+      <c r="I1150">
+        <v>0</v>
+      </c>
+      <c r="J1150" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="1151" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1151" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1151" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1151" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1151" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1151">
+        <v>8</v>
+      </c>
+      <c r="F1151" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1151" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1151">
+        <v>0.375</v>
+      </c>
+      <c r="I1151">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="1152" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1152" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1152" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1152" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1152" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1152">
+        <v>4</v>
+      </c>
+      <c r="F1152" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1152" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1152">
+        <v>0.25</v>
+      </c>
+      <c r="I1152">
+        <v>0</v>
+      </c>
+      <c r="J1152" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="1153" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1153" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1153" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1153" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1153" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1153">
+        <v>8</v>
+      </c>
+      <c r="F1153" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1153" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1153">
+        <v>0.375</v>
+      </c>
+      <c r="I1153">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="1154" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1154" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1154" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1154" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1154" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1154">
+        <v>4</v>
+      </c>
+      <c r="F1154" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1154" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1154">
+        <v>0.25</v>
+      </c>
+      <c r="I1154">
+        <v>0</v>
+      </c>
+      <c r="J1154" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="1155" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1155" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1155" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1155" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1155" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1155">
+        <v>8</v>
+      </c>
+      <c r="F1155" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1155" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1155">
+        <v>0.375</v>
+      </c>
+      <c r="I1155">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="1156" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1156" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1156" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1156" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1156" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1156">
+        <v>4</v>
+      </c>
+      <c r="F1156" t="s">
+        <v>247</v>
+      </c>
+      <c r="G1156" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1156">
+        <v>0</v>
+      </c>
+      <c r="I1156">
+        <v>0</v>
+      </c>
+      <c r="J1156" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="1157" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1157" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1157" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1157" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1157" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1157">
+        <v>8</v>
+      </c>
+      <c r="F1157" t="s">
+        <v>247</v>
+      </c>
+      <c r="G1157" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1157">
+        <v>0.5</v>
+      </c>
+      <c r="I1157">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="1158" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1158" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1158" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1158" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1158" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1158">
+        <v>4</v>
+      </c>
+      <c r="F1158" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1158" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1158">
+        <v>0.25</v>
+      </c>
+      <c r="I1158">
+        <v>0</v>
+      </c>
+      <c r="J1158" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="1159" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1159" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1159" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1159" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1159" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1159">
+        <v>8</v>
+      </c>
+      <c r="F1159" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1159" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1159">
+        <v>0.125</v>
+      </c>
+      <c r="I1159">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="1160" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1160" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1160" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1160" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1160" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1160">
+        <v>4</v>
+      </c>
+      <c r="F1160" t="s">
+        <v>234</v>
+      </c>
+      <c r="G1160" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1160">
+        <v>0</v>
+      </c>
+      <c r="I1160">
+        <v>0</v>
+      </c>
+      <c r="J1160" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="1161" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1161" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1161" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1161" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1161" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1161">
+        <v>8</v>
+      </c>
+      <c r="F1161" t="s">
+        <v>234</v>
+      </c>
+      <c r="G1161" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1161">
+        <v>0.25</v>
+      </c>
+      <c r="I1161">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="1162" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1162" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1162" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1162" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1162" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1162">
+        <v>4</v>
+      </c>
+      <c r="F1162" t="s">
+        <v>233</v>
+      </c>
+      <c r="G1162" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1162">
+        <v>0.25</v>
+      </c>
+      <c r="I1162">
+        <v>0</v>
+      </c>
+      <c r="J1162" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="1163" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1163" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1163" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1163" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1163" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1163">
+        <v>8</v>
+      </c>
+      <c r="F1163" t="s">
+        <v>233</v>
+      </c>
+      <c r="G1163" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1163">
+        <v>0.125</v>
+      </c>
+      <c r="I1163">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="1164" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1164" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1164" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1164" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1164" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1164">
+        <v>4</v>
+      </c>
+      <c r="F1164" t="s">
+        <v>263</v>
+      </c>
+      <c r="G1164" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1164">
+        <v>0</v>
+      </c>
+      <c r="I1164">
+        <v>0</v>
+      </c>
+      <c r="J1164" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="1165" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1165" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1165" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1165" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1165" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1165">
+        <v>8</v>
+      </c>
+      <c r="F1165" t="s">
+        <v>263</v>
+      </c>
+      <c r="G1165" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1165">
+        <v>0.25</v>
+      </c>
+      <c r="I1165">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="1166" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1166" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1166" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1166" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1166" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1166">
+        <v>4</v>
+      </c>
+      <c r="F1166" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1166" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1166">
+        <v>0.25</v>
+      </c>
+      <c r="I1166">
+        <v>0</v>
+      </c>
+      <c r="J1166" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="1167" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1167" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1167" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1167" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1167" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1167">
+        <v>8</v>
+      </c>
+      <c r="F1167" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1167" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1167">
+        <v>0.125</v>
+      </c>
+      <c r="I1167">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="1168" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1168" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1168" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1168" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1168" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1168">
+        <v>4</v>
+      </c>
+      <c r="F1168" t="s">
+        <v>194</v>
+      </c>
+      <c r="G1168" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1168">
+        <v>0</v>
+      </c>
+      <c r="I1168">
+        <v>0</v>
+      </c>
+      <c r="J1168" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="1169" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1169" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1169" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1169" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1169" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1169">
+        <v>8</v>
+      </c>
+      <c r="F1169" t="s">
+        <v>194</v>
+      </c>
+      <c r="G1169" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1169">
+        <v>0.125</v>
+      </c>
+      <c r="I1169">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="1170" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1170" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1170" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1170" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1170" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1170">
+        <v>4</v>
+      </c>
+      <c r="F1170" t="s">
+        <v>278</v>
+      </c>
+      <c r="G1170" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1170">
+        <v>0</v>
+      </c>
+      <c r="I1170">
+        <v>0</v>
+      </c>
+      <c r="J1170" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="1171" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1171" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1171" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1171" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1171" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1171">
+        <v>8</v>
+      </c>
+      <c r="F1171" t="s">
+        <v>278</v>
+      </c>
+      <c r="G1171" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1171">
+        <v>0.125</v>
+      </c>
+      <c r="I1171">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="1172" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1172" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1172" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1172" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1172" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1172">
+        <v>4</v>
+      </c>
+      <c r="F1172" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1172" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1172">
+        <v>0</v>
+      </c>
+      <c r="I1172">
+        <v>0</v>
+      </c>
+      <c r="J1172" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="1173" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1173" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1173" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1173" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1173" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1173">
+        <v>8</v>
+      </c>
+      <c r="F1173" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1173" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1173">
+        <v>0.125</v>
+      </c>
+      <c r="I1173">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="1174" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1174" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1174" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1174" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1174" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1174">
+        <v>4</v>
+      </c>
+      <c r="F1174" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1174" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1174">
+        <v>0</v>
+      </c>
+      <c r="I1174">
+        <v>0</v>
+      </c>
+      <c r="J1174" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="1175" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1175" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1175" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1175" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1175" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1175">
+        <v>8</v>
+      </c>
+      <c r="F1175" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1175" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1175">
+        <v>0.125</v>
+      </c>
+      <c r="I1175">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="1176" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1176" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1176" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1176" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1176" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1176">
+        <v>4</v>
+      </c>
+      <c r="F1176" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1176" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1176">
+        <v>0</v>
+      </c>
+      <c r="I1176">
+        <v>0</v>
+      </c>
+      <c r="J1176" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="1177" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1177" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1177" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1177" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1177" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1177">
+        <v>8</v>
+      </c>
+      <c r="F1177" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1177" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1177">
+        <v>0.125</v>
+      </c>
+      <c r="I1177">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="1178" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1178" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1178" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1178" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1178" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1178">
+        <v>4</v>
+      </c>
+      <c r="F1178" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1178" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1178">
+        <v>0</v>
+      </c>
+      <c r="I1178">
+        <v>0</v>
+      </c>
+      <c r="J1178" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="1179" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1179" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1179" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1179" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1179" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1179">
+        <v>8</v>
+      </c>
+      <c r="F1179" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1179" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1179">
+        <v>0.125</v>
+      </c>
+      <c r="I1179">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="1180" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1180" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1180" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1180" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1180" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1180">
+        <v>4</v>
+      </c>
+      <c r="F1180" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1180" t="s">
+        <v>277</v>
+      </c>
+      <c r="H1180">
+        <v>0.25</v>
+      </c>
+      <c r="I1180">
+        <v>0</v>
+      </c>
+      <c r="J1180" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="1181" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1181" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1181" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1181" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1181" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1181">
+        <v>8</v>
+      </c>
+      <c r="F1181" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1181" t="s">
+        <v>277</v>
+      </c>
+      <c r="H1181">
+        <v>0.125</v>
+      </c>
+      <c r="I1181">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="1182" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1182" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1182" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1182" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1182" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1182">
+        <v>4</v>
+      </c>
+      <c r="F1182" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1182" t="s">
+        <v>277</v>
+      </c>
+      <c r="H1182">
+        <v>0</v>
+      </c>
+      <c r="I1182">
+        <v>0</v>
+      </c>
+      <c r="J1182" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="1183" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1183" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1183" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1183" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1183" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1183">
+        <v>8</v>
+      </c>
+      <c r="F1183" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1183" t="s">
+        <v>277</v>
+      </c>
+      <c r="H1183">
+        <v>0.5</v>
+      </c>
+      <c r="I1183">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="1184" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1184" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1184" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1184" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1184" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1184">
+        <v>4</v>
+      </c>
+      <c r="F1184" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1184" t="s">
+        <v>277</v>
+      </c>
+      <c r="H1184">
+        <v>0.25</v>
+      </c>
+      <c r="I1184">
+        <v>0</v>
+      </c>
+      <c r="J1184" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="1185" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1185" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1185" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1185" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1185" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1185">
+        <v>8</v>
+      </c>
+      <c r="F1185" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1185" t="s">
+        <v>277</v>
+      </c>
+      <c r="H1185">
+        <v>0</v>
+      </c>
+      <c r="I1185">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="1186" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1186" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1186" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1186" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1186" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1186">
+        <v>4</v>
+      </c>
+      <c r="F1186" t="s">
+        <v>194</v>
+      </c>
+      <c r="G1186" t="s">
+        <v>277</v>
+      </c>
+      <c r="H1186">
+        <v>0</v>
+      </c>
+      <c r="I1186">
+        <v>0</v>
+      </c>
+      <c r="J1186" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="1187" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1187" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1187" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1187" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1187" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1187">
+        <v>8</v>
+      </c>
+      <c r="F1187" t="s">
+        <v>194</v>
+      </c>
+      <c r="G1187" t="s">
+        <v>277</v>
+      </c>
+      <c r="H1187">
+        <v>0.125</v>
+      </c>
+      <c r="I1187">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="1188" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1188" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1188" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1188" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1188" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1188">
+        <v>4</v>
+      </c>
+      <c r="F1188" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1188" t="s">
+        <v>277</v>
+      </c>
+      <c r="H1188">
+        <v>0.5</v>
+      </c>
+      <c r="I1188">
+        <v>0</v>
+      </c>
+      <c r="J1188" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="1189" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1189" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1189" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1189" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1189" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1189">
+        <v>8</v>
+      </c>
+      <c r="F1189" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1189" t="s">
+        <v>277</v>
+      </c>
+      <c r="H1189">
+        <v>0.625</v>
+      </c>
+      <c r="I1189">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="1190" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1190" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1190" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1190" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1190" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1190">
+        <v>4</v>
+      </c>
+      <c r="F1190" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1190" t="s">
+        <v>277</v>
+      </c>
+      <c r="H1190">
+        <v>0.25</v>
+      </c>
+      <c r="I1190">
+        <v>0</v>
+      </c>
+      <c r="J1190" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="1191" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1191" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1191" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1191" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1191" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1191">
+        <v>8</v>
+      </c>
+      <c r="F1191" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1191" t="s">
+        <v>277</v>
+      </c>
+      <c r="H1191">
+        <v>0.625</v>
+      </c>
+      <c r="I1191">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="1192" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1192" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1192" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1192" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1192" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1192">
+        <v>4</v>
+      </c>
+      <c r="F1192" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1192" t="s">
+        <v>277</v>
+      </c>
+      <c r="H1192">
+        <v>0.25</v>
+      </c>
+      <c r="I1192">
+        <v>0</v>
+      </c>
+      <c r="J1192" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="1193" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1193" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1193" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1193" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1193" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1193">
+        <v>8</v>
+      </c>
+      <c r="F1193" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1193" t="s">
+        <v>277</v>
+      </c>
+      <c r="H1193">
+        <v>0.125</v>
+      </c>
+      <c r="I1193">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="1194" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1194" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1194" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1194" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1194" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1194">
+        <v>4</v>
+      </c>
+      <c r="F1194" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1194" t="s">
+        <v>277</v>
+      </c>
+      <c r="H1194">
+        <v>0</v>
+      </c>
+      <c r="I1194">
+        <v>0</v>
+      </c>
+      <c r="J1194" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="1195" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1195" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1195" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1195" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1195" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1195">
+        <v>8</v>
+      </c>
+      <c r="F1195" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1195" t="s">
+        <v>277</v>
+      </c>
+      <c r="H1195">
+        <v>0.125</v>
+      </c>
+      <c r="I1195">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="1196" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1196" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1196" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1196" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1196" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1196">
+        <v>4</v>
+      </c>
+      <c r="F1196" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1196" t="s">
+        <v>277</v>
+      </c>
+      <c r="H1196">
+        <v>0.25</v>
+      </c>
+      <c r="I1196">
+        <v>0</v>
+      </c>
+      <c r="J1196" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="1197" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1197" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1197" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1197" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1197" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1197">
+        <v>8</v>
+      </c>
+      <c r="F1197" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1197" t="s">
+        <v>277</v>
+      </c>
+      <c r="H1197">
+        <v>0</v>
+      </c>
+      <c r="I1197">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="1198" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1198" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1198" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1198" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1198" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1198">
+        <v>4</v>
+      </c>
+      <c r="F1198" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1198" t="s">
+        <v>277</v>
+      </c>
+      <c r="H1198">
+        <v>0</v>
+      </c>
+      <c r="I1198">
+        <v>0</v>
+      </c>
+      <c r="J1198" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="1199" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1199" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1199" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1199" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1199" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1199">
+        <v>8</v>
+      </c>
+      <c r="F1199" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1199" t="s">
+        <v>277</v>
+      </c>
+      <c r="H1199">
+        <v>0.375</v>
+      </c>
+      <c r="I1199">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="1200" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1200" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1200" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1200" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1200" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1200">
+        <v>4</v>
+      </c>
+      <c r="F1200" t="s">
+        <v>234</v>
+      </c>
+      <c r="G1200" t="s">
+        <v>277</v>
+      </c>
+      <c r="H1200">
+        <v>0.5</v>
+      </c>
+      <c r="I1200">
+        <v>0</v>
+      </c>
+      <c r="J1200" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="1201" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1201" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1201" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1201" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1201" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1201">
+        <v>8</v>
+      </c>
+      <c r="F1201" t="s">
+        <v>234</v>
+      </c>
+      <c r="G1201" t="s">
+        <v>277</v>
+      </c>
+      <c r="H1201">
+        <v>0.5</v>
+      </c>
+      <c r="I1201">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="1202" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1202" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1202" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1202" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1202" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1202">
+        <v>4</v>
+      </c>
+      <c r="F1202" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1202" t="s">
+        <v>277</v>
+      </c>
+      <c r="H1202">
+        <v>0.5</v>
+      </c>
+      <c r="I1202">
+        <v>0</v>
+      </c>
+      <c r="J1202" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="1203" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1203" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1203" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1203" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1203" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1203">
+        <v>8</v>
+      </c>
+      <c r="F1203" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1203" t="s">
+        <v>277</v>
+      </c>
+      <c r="H1203">
+        <v>0.375</v>
+      </c>
+      <c r="I1203">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="1204" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1204" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1204" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1204" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1204" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1204">
+        <v>4</v>
+      </c>
+      <c r="F1204" t="s">
+        <v>172</v>
+      </c>
+      <c r="G1204" t="s">
+        <v>277</v>
+      </c>
+      <c r="H1204">
+        <v>0</v>
+      </c>
+      <c r="I1204">
+        <v>0</v>
+      </c>
+      <c r="J1204" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="1205" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1205" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1205" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1205" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1205" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1205">
+        <v>8</v>
+      </c>
+      <c r="F1205" t="s">
+        <v>172</v>
+      </c>
+      <c r="G1205" t="s">
+        <v>277</v>
+      </c>
+      <c r="H1205">
+        <v>0.125</v>
+      </c>
+      <c r="I1205">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="1206" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1206" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1206" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1206" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1206" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1206">
+        <v>4</v>
+      </c>
+      <c r="F1206" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1206" t="s">
+        <v>277</v>
+      </c>
+      <c r="H1206">
+        <v>0.25</v>
+      </c>
+      <c r="I1206">
+        <v>0</v>
+      </c>
+      <c r="J1206" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="1207" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1207" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1207" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1207" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1207" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1207">
+        <v>8</v>
+      </c>
+      <c r="F1207" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1207" t="s">
+        <v>277</v>
+      </c>
+      <c r="H1207">
+        <v>0</v>
+      </c>
+      <c r="I1207">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="1208" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1208" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1208" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1208" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1208" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1208">
+        <v>4</v>
+      </c>
+      <c r="F1208" t="s">
+        <v>247</v>
+      </c>
+      <c r="G1208" t="s">
+        <v>277</v>
+      </c>
+      <c r="H1208">
+        <v>0.25</v>
+      </c>
+      <c r="I1208">
+        <v>0</v>
+      </c>
+      <c r="J1208" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="1209" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1209" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1209" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1209" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1209" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1209">
+        <v>8</v>
+      </c>
+      <c r="F1209" t="s">
+        <v>247</v>
+      </c>
+      <c r="G1209" t="s">
+        <v>277</v>
+      </c>
+      <c r="H1209">
+        <v>0</v>
+      </c>
+      <c r="I1209">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="1210" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1210" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1210" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1210" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1210" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1210">
+        <v>4</v>
+      </c>
+      <c r="F1210" t="s">
+        <v>263</v>
+      </c>
+      <c r="G1210" t="s">
+        <v>277</v>
+      </c>
+      <c r="H1210">
+        <v>0</v>
+      </c>
+      <c r="I1210">
+        <v>0</v>
+      </c>
+      <c r="J1210" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="1211" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1211" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1211" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1211" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1211" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1211">
+        <v>8</v>
+      </c>
+      <c r="F1211" t="s">
+        <v>263</v>
+      </c>
+      <c r="G1211" t="s">
+        <v>277</v>
+      </c>
+      <c r="H1211">
+        <v>0.125</v>
+      </c>
+      <c r="I1211">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="1212" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1212" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1212" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1212" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1212" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1212">
+        <v>4</v>
+      </c>
+      <c r="F1212" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1212" t="s">
+        <v>277</v>
+      </c>
+      <c r="H1212">
+        <v>0.25</v>
+      </c>
+      <c r="I1212">
+        <v>0</v>
+      </c>
+      <c r="J1212" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="1213" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1213" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1213" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1213" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1213" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1213">
+        <v>8</v>
+      </c>
+      <c r="F1213" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1213" t="s">
+        <v>277</v>
+      </c>
+      <c r="H1213">
+        <v>0.125</v>
+      </c>
+      <c r="I1213">
+        <v>75</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>